<commit_message>
[BugFixing] MonsterPosList ParseVector2int 에서 오류 발견
</commit_message>
<xml_diff>
--- a/Assets/PSW/Excel/StageMap.xlsx
+++ b/Assets/PSW/Excel/StageMap.xlsx
@@ -57,21 +57,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-0,0,0,0,0,0,
-0,1,0,0,0,0,
-0,1,0,0,0,0,
-0,1,1,1,1,0,
-0,0,0,0,1,0,
-0,0,0,0,0,0
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{{4,4}}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -81,6 +66,14 @@
   </si>
   <si>
     <t>{UIUpMoveBlock,UIDownMoveBlock,UILeftMoveBlock,UIRightMoveBlock,UIWaterAttackBlock,UIGrassAttackBlock,UIFireAttackBlock}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0,0,0,0,0,0,0,1,0,0,0,0,0,1,0,0,0,0,0,1,1,1,1,0,0,0,0,0,1,0,0,0,0,0,0,0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BlueMonster}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -412,7 +405,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -452,7 +445,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="132" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -460,22 +453,22 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Update] Loop, Condition 로직수정중
</commit_message>
<xml_diff>
--- a/Assets/PSW/Excel/StageMap.xlsx
+++ b/Assets/PSW/Excel/StageMap.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>StageIndex</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,6 +74,10 @@
   </si>
   <si>
     <t>{(4/4)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bushmonsternamelist</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -402,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -414,12 +418,13 @@
     <col min="2" max="2" width="11.75" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="20.75" customWidth="1"/>
+    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="23.375" customWidth="1"/>
+    <col min="9" max="9" width="24.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,8 +449,11 @@
       <c r="H1" t="s">
         <v>4</v>
       </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>